<commit_message>
Completed the verification of a traffic light system with 100% code coverage and functional coverage.
</commit_message>
<xml_diff>
--- a/verification plan/verification plan.xlsx
+++ b/verification plan/verification plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shared Folders\Uni\courses\Digital circuit\digital github codes\Done\Traffic Light\verification plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shared Folders\Uni\courses\Digital circuit\digital github codes\Done\Traffic Light\Traffic-light-UVM\verification plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367131F7-C9B4-4DB8-8D9E-044EE5A54746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54688674-70AE-4EB4-BCC0-8C173EB5E87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BE33C207-AC50-49BB-BEDD-1F59C983F64D}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="15450" xr2:uid="{BE33C207-AC50-49BB-BEDD-1F59C983F64D}"/>
   </bookViews>
   <sheets>
     <sheet name="Verification Plan" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t>#</t>
   </si>
@@ -83,21 +83,12 @@
     <t>Coverpoint</t>
   </si>
   <si>
-    <t>Reset Behavior</t>
-  </si>
-  <si>
     <t>c_preset_distribution</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>Cover reset transitions</t>
   </si>
   <si>
-    <t>tl_cov_grp::rst_cp</t>
-  </si>
-  <si>
     <t>FSM design</t>
   </si>
   <si>
@@ -107,15 +98,9 @@
     <t>Smart System feature 2</t>
   </si>
   <si>
-    <t>Light algorithm</t>
-  </si>
-  <si>
     <t>Smart System feature 3</t>
   </si>
   <si>
-    <t>Cover FSM transtions &amp; States</t>
-  </si>
-  <si>
     <t>Reset Inactive Distribution</t>
   </si>
   <si>
@@ -125,18 +110,9 @@
     <t>Apply a 97% probability of LOW and 3% probability of HIGH</t>
   </si>
   <si>
-    <t>Main Street Priority</t>
-  </si>
-  <si>
-    <t>Ensure that the main street (road A) gets the green light immediately after a reset, confirming priority</t>
-  </si>
-  <si>
     <t>Ensure that the auto-generated FSM design matches the specification</t>
   </si>
   <si>
-    <t>Ensure the system returns to its default state when the reset is asserted, and all internal signals are deasserted (e.g., Ra_tmp, Rb_tmp, Ga_tmp, Gb_tmp, Ya_tmp, Yb_tmp set to 0)</t>
-  </si>
-  <si>
     <t>Road B Green Light Activation</t>
   </si>
   <si>
@@ -165,6 +141,56 @@
   </si>
   <si>
     <t>Cover the reset transitions HIGH→ LOW, LOW→ HIGH</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Reset Behavior &amp; Main Street Priority</t>
+  </si>
+  <si>
+    <t>Ensure the system returns to its default state when the reset is asserted, and all output signals are deasserted (e.g., Ra, Rb, Ga, Gb, Ya, Yb set to 0)
+Ensure that the main street (road A) gets the green light immediately after a reset, confirming priority  (e.g., Rb, Ga, set to 1)</t>
+  </si>
+  <si>
+    <t>road_B_green_assert</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>road_A_priority_assert</t>
+  </si>
+  <si>
+    <t>smart_system_feature_1_assert</t>
+  </si>
+  <si>
+    <t>smart_system_feature_2_assert</t>
+  </si>
+  <si>
+    <t>smart_system_feature_3_assert</t>
+  </si>
+  <si>
+    <t>traffic_cov_grp::rst_cp</t>
+  </si>
+  <si>
+    <t>Cover Directive</t>
+  </si>
+  <si>
+    <t>light_algorithm_A_cover
+light_algorithm_B_cover</t>
+  </si>
+  <si>
+    <t>FSM Coverage</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>Light Algorithm</t>
+  </si>
+  <si>
+    <t>Cover FSM Ttranstions &amp; States</t>
   </si>
 </sst>
 </file>
@@ -348,23 +374,23 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -710,11 +736,11 @@
     <tabColor theme="3" tint="0.249977111117893"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25"/>
@@ -732,7 +758,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" ht="21.75">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -756,12 +782,12 @@
       <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="22" customFormat="1">
-      <c r="A2" s="26">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -773,17 +799,17 @@
       <c r="F2" s="10"/>
       <c r="G2" s="7"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" spans="1:13" ht="72">
-      <c r="A3" s="30">
+      <c r="I2" s="32"/>
+    </row>
+    <row r="3" spans="1:13" ht="108">
+      <c r="A3" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>32</v>
+        <v>36</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>37</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>11</v>
@@ -791,35 +817,37 @@
       <c r="E3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="32"/>
+      <c r="F3" s="29" t="s">
+        <v>39</v>
+      </c>
       <c r="G3" s="12">
         <v>1</v>
       </c>
       <c r="H3" s="15">
         <v>100</v>
       </c>
-      <c r="I3" s="16" t="s">
-        <v>17</v>
+      <c r="I3" s="20" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="36">
-      <c r="A4" s="30">
+      <c r="A4" s="24">
         <v>1.2</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>27</v>
+        <v>21</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>22</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="32" t="s">
-        <v>28</v>
+      <c r="F4" s="29" t="s">
+        <v>23</v>
       </c>
       <c r="G4" s="12">
         <v>1</v>
@@ -827,40 +855,42 @@
       <c r="H4" s="15">
         <v>100</v>
       </c>
-      <c r="I4" s="16" t="s">
-        <v>17</v>
+      <c r="I4" s="20" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="36">
-      <c r="A5" s="29">
+      <c r="A5" s="33">
         <v>1.3</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>42</v>
+        <v>16</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>34</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="E5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="29" t="s">
+        <v>39</v>
+      </c>
       <c r="G5" s="12">
         <v>1</v>
       </c>
       <c r="H5" s="15">
         <v>100</v>
       </c>
-      <c r="I5" s="16" t="s">
-        <v>17</v>
+      <c r="I5" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="M5" s="23"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="26">
+      <c r="A6" s="7">
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -872,201 +902,242 @@
       <c r="F6" s="15"/>
       <c r="G6" s="12"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="16"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7" spans="1:13" ht="36">
-      <c r="A7" s="29">
+      <c r="A7" s="33">
         <v>2.1</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="14"/>
+        <v>24</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>39</v>
+      </c>
       <c r="E7" s="12"/>
-      <c r="F7" s="15"/>
+      <c r="F7" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="G7" s="12">
         <v>1</v>
       </c>
       <c r="H7" s="15">
         <v>100</v>
       </c>
-      <c r="I7" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="36">
-      <c r="A8" s="30">
+      <c r="I7" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="54">
+      <c r="A8" s="24">
         <v>2.2000000000000002</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="15"/>
+        <v>26</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="G8" s="12">
         <v>1</v>
       </c>
       <c r="H8" s="15">
         <v>100</v>
       </c>
-      <c r="I8" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="54">
-      <c r="A9" s="30">
+      <c r="I8" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="72">
+      <c r="A9" s="7">
         <v>2.2999999999999998</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="15"/>
+        <v>28</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="G9" s="12">
         <v>1</v>
       </c>
       <c r="H9" s="15">
         <v>100</v>
       </c>
-      <c r="I9" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="72">
-      <c r="A10" s="30">
+      <c r="I9" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="54">
+      <c r="A10" s="33">
         <v>2.4</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="15"/>
+        <v>30</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="G10" s="12">
         <v>1</v>
       </c>
       <c r="H10" s="15">
         <v>100</v>
       </c>
-      <c r="I10" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="54">
-      <c r="A11" s="30">
+      <c r="I10" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="36">
+      <c r="A11" s="24">
         <v>2.5</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="15"/>
+        <v>29</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="G11" s="12">
         <v>1</v>
       </c>
       <c r="H11" s="15">
         <v>100</v>
       </c>
-      <c r="I11" s="16" t="s">
-        <v>17</v>
+      <c r="I11" s="20" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="36">
-      <c r="A12" s="30">
+      <c r="A12" s="7">
         <v>2.6</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="15"/>
+        <v>31</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="G12" s="12">
         <v>1</v>
       </c>
       <c r="H12" s="15">
         <v>100</v>
       </c>
-      <c r="I12" s="16" t="s">
-        <v>17</v>
+      <c r="I12" s="20" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="36">
-      <c r="A13" s="29">
+      <c r="A13" s="33">
         <v>2.7</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="C13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="F13" s="14"/>
       <c r="G13" s="12">
         <v>1</v>
       </c>
       <c r="H13" s="15">
         <v>100</v>
       </c>
-      <c r="I13" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="36">
-      <c r="A14" s="30">
+      <c r="I13" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="54">
+      <c r="A14" s="24">
         <v>2.8</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="15"/>
+        <v>32</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="G14" s="12">
         <v>1</v>
       </c>
       <c r="H14" s="15">
         <v>100</v>
       </c>
-      <c r="I14" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="54">
-      <c r="A15" s="30">
-        <v>2.9</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>40</v>
-      </c>
+      <c r="I14" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="26"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="14"/>
       <c r="E15" s="12"/>
       <c r="F15" s="15"/>
@@ -1087,24 +1158,24 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="26"/>
-      <c r="B17" s="8"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="12"/>
       <c r="F17" s="15"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="15"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="21"/>
       <c r="I17" s="16"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="26"/>
-      <c r="B18" s="19"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="13"/>
-      <c r="D18" s="18"/>
+      <c r="D18" s="14"/>
       <c r="E18" s="12"/>
       <c r="F18" s="15"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="21"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="15"/>
       <c r="I18" s="16"/>
     </row>
     <row r="19" spans="1:9">
@@ -1120,24 +1191,24 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="26"/>
-      <c r="B20" s="8"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="12"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="15"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
       <c r="I20" s="16"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="26"/>
-      <c r="B21" s="19"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="13"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="20"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="12"/>
       <c r="F21" s="15"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="21"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="15"/>
       <c r="I21" s="16"/>
     </row>
     <row r="22" spans="1:9">
@@ -1153,21 +1224,21 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="26"/>
-      <c r="B23" s="8"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="13"/>
       <c r="D23" s="14"/>
       <c r="E23" s="12"/>
       <c r="F23" s="15"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="15"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
       <c r="I23" s="16"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="26"/>
       <c r="B24" s="19"/>
       <c r="C24" s="13"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="12"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="15"/>
       <c r="G24" s="20"/>
       <c r="H24" s="21"/>
@@ -1200,7 +1271,7 @@
       <c r="B27" s="19"/>
       <c r="C27" s="13"/>
       <c r="D27" s="18"/>
-      <c r="E27" s="20"/>
+      <c r="E27" s="12"/>
       <c r="F27" s="15"/>
       <c r="G27" s="20"/>
       <c r="H27" s="21"/>
@@ -1219,10 +1290,10 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="26"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="12"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="15"/>
       <c r="G29" s="20"/>
       <c r="H29" s="21"/>
@@ -1230,10 +1301,10 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="26"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="20"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="12"/>
       <c r="F30" s="15"/>
       <c r="G30" s="20"/>
       <c r="H30" s="21"/>
@@ -1265,7 +1336,7 @@
       <c r="A33" s="26"/>
       <c r="B33" s="19"/>
       <c r="C33" s="13"/>
-      <c r="D33" s="18"/>
+      <c r="D33" s="14"/>
       <c r="E33" s="12"/>
       <c r="F33" s="15"/>
       <c r="G33" s="20"/>
@@ -1276,23 +1347,15 @@
       <c r="A34" s="26"/>
       <c r="B34" s="19"/>
       <c r="C34" s="13"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="12"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="20"/>
       <c r="F34" s="15"/>
       <c r="G34" s="20"/>
       <c r="H34" s="21"/>
       <c r="I34" s="16"/>
     </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="26"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="16"/>
+    <row r="36" spans="1:9">
+      <c r="A36" s="26"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="26"/>
@@ -1314,9 +1377,6 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="26"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>